<commit_message>
added data in xlsx and csv
</commit_message>
<xml_diff>
--- a/TEO-events.xlsx
+++ b/TEO-events.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="154">
   <si>
     <t>cod_event</t>
   </si>
@@ -25,226 +25,454 @@
     <t>event_type</t>
   </si>
   <si>
+    <t>cod_prerequisites</t>
+  </si>
+  <si>
+    <t>IM853</t>
+  </si>
+  <si>
+    <t>CIRCUITOS DIGITAIS</t>
+  </si>
+  <si>
+    <t>MANDATORY</t>
+  </si>
+  <si>
+    <t>IM885</t>
+  </si>
+  <si>
+    <t>GEOMETRIA ANALÍTICA</t>
+  </si>
+  <si>
+    <t>TN703</t>
+  </si>
+  <si>
     <t>COMPUTADORES E SOCIEDADE</t>
   </si>
   <si>
-    <t>MANDATORY</t>
+    <t>TN705</t>
+  </si>
+  <si>
+    <t>MATEMÁTICA DISCRETA PARA COMPUTAÇÃO</t>
+  </si>
+  <si>
+    <t>TN706</t>
   </si>
   <si>
     <t>PROGRAMAÇÃO ESTRUTURADA</t>
   </si>
   <si>
-    <t>GEOMETRIA ANALÍTICA</t>
+    <t>TN707</t>
   </si>
   <si>
     <t>INTRODUÇÃO À CIÊNCIA DA COMPUTAÇÃO</t>
   </si>
   <si>
-    <t>MATEMÁTICA DISCRETA PARA COMPUTAÇÃO</t>
-  </si>
-  <si>
-    <t>CIRCUITOS DIGITAIS</t>
+    <t>IM403</t>
   </si>
   <si>
     <t>CÁLCULO I</t>
   </si>
   <si>
+    <t>IM429</t>
+  </si>
+  <si>
+    <t>ÁLGEBRA LINEAR I</t>
+  </si>
+  <si>
+    <t>TN709</t>
+  </si>
+  <si>
+    <t>LÓGICA PARA COMPUTAÇÃO</t>
+  </si>
+  <si>
+    <t>TN710</t>
+  </si>
+  <si>
     <t>ENGENHARIA DE SOFTWARE I</t>
   </si>
   <si>
-    <t>ÁLGEBRA LINEAR I</t>
+    <t>TN711</t>
   </si>
   <si>
     <t>ESTRUTURA DE DADOS I</t>
   </si>
   <si>
-    <t>LÓGICA PARA COMPUTAÇÃO</t>
+    <t>TN712</t>
   </si>
   <si>
     <t>ARQUITETURA DE COMPUTADORES</t>
   </si>
   <si>
+    <t>IM404</t>
+  </si>
+  <si>
     <t>CÁLCULO II</t>
   </si>
   <si>
+    <t>IM478</t>
+  </si>
+  <si>
+    <t>ÁLGEBRA LINEAR COMPUTACIONAL</t>
+  </si>
+  <si>
+    <t>TN715</t>
+  </si>
+  <si>
+    <t>LINGUAGENS FORMAIS E AUTÔMATOS</t>
+  </si>
+  <si>
+    <t>TN716</t>
+  </si>
+  <si>
     <t>MODELAGEM E PROJETO DE SOFTWARE</t>
   </si>
   <si>
-    <t>ÁLGEBRA LINEAR COMPUTACIONAL</t>
+    <t>TN717</t>
   </si>
   <si>
     <t>PROGRAMAÇÃO ORIENTADA A OBJETOS</t>
   </si>
   <si>
-    <t>LINGUAGENS FORMAIS E AUTÔMATOS</t>
+    <t>TN718</t>
   </si>
   <si>
     <t>GRAFOS E ALGORITMOS</t>
   </si>
   <si>
+    <t>IM859</t>
+  </si>
+  <si>
+    <t>PROBABILIDADE E ESTATÍSTICA PARA CIÊNCIA DA COMPUTAÇÃO</t>
+  </si>
+  <si>
+    <t>IM868</t>
+  </si>
+  <si>
+    <t>SISTEMAS OPERACIONAIS</t>
+  </si>
+  <si>
+    <t>TM406</t>
+  </si>
+  <si>
     <t>CÁLCULO III</t>
   </si>
   <si>
-    <t>SISTEMAS OPERACIONAIS</t>
+    <t>TM407</t>
+  </si>
+  <si>
+    <t>FÍSICA PARA CIÊNCIA DA COMPUTAÇÃO</t>
+  </si>
+  <si>
+    <t>TN720</t>
   </si>
   <si>
     <t>LINGUAGENS DE PROGRAMAÇÃO</t>
   </si>
   <si>
-    <t>FÍSICA PARA CIÊNCIA DA COMPUTAÇÃO</t>
-  </si>
-  <si>
-    <t>PROBABILIDADE E ESTATÍSTICA PARA CIÊNCIA DA COMPUTAÇÃO</t>
+    <t>TN723</t>
   </si>
   <si>
     <t>ANÁLISE E PROJETO DE ALGORITMOS</t>
   </si>
   <si>
+    <t>TM421</t>
+  </si>
+  <si>
+    <t>COMPUTAÇÃO GRÁFICA</t>
+  </si>
+  <si>
+    <t>IM429,TN711</t>
+  </si>
+  <si>
+    <t>TN724</t>
+  </si>
+  <si>
     <t>INTELIGÊNCIA ARTIFICIAL</t>
   </si>
   <si>
+    <t>TN711,TN709</t>
+  </si>
+  <si>
+    <t>TN725</t>
+  </si>
+  <si>
+    <t>COMPILADORES</t>
+  </si>
+  <si>
+    <t>TN715,TN720</t>
+  </si>
+  <si>
+    <t>TN726</t>
+  </si>
+  <si>
+    <t>MÉTODOS NUMÉRICOS</t>
+  </si>
+  <si>
+    <t>TN727</t>
+  </si>
+  <si>
     <t>BANCO DE DADOS</t>
   </si>
   <si>
-    <t>COMPILADORES</t>
-  </si>
-  <si>
-    <t>COMPUTAÇÃO GRÁFICA</t>
-  </si>
-  <si>
-    <t>MÉTODOS NUMÉRICOS</t>
+    <t>TN728</t>
   </si>
   <si>
     <t>OTIMIZAÇÃO LINEAR</t>
   </si>
   <si>
+    <t>TN729</t>
+  </si>
+  <si>
     <t>REDES E SISTEMAS DISTRIBUÍDOS</t>
   </si>
   <si>
+    <t>TN730</t>
+  </si>
+  <si>
     <t>ESTRUTURA DE DADOS 2</t>
   </si>
   <si>
+    <t>IM188</t>
+  </si>
+  <si>
+    <t>CULTURA AFRO-BRASILEIRA E AFRICANA</t>
+  </si>
+  <si>
+    <t>OPTIONAL</t>
+  </si>
+  <si>
+    <t>IM461</t>
+  </si>
+  <si>
     <t>LINGUAGEM BRASILEIRA DE SINAIS (LIBRAS)</t>
   </si>
   <si>
-    <t>OPTIONAL</t>
-  </si>
-  <si>
-    <t>CULTURA AFRO-BRASILEIRA E AFRICANA</t>
+    <t>TM419</t>
+  </si>
+  <si>
+    <t>GERÊNCIA DE PROJETOS</t>
+  </si>
+  <si>
+    <t>TM429</t>
+  </si>
+  <si>
+    <t>INTRODUÇÃO À TEORIA DOS SISTEMAS DE RECOMENDAÇÃO</t>
+  </si>
+  <si>
+    <t>TM430</t>
+  </si>
+  <si>
+    <t>REDES DE COMPUTADORES SEM FIO</t>
+  </si>
+  <si>
+    <t>TM431</t>
+  </si>
+  <si>
+    <t>INTRODUÇÃO À TEORIA DAS REDES DE PETRI</t>
+  </si>
+  <si>
+    <t>TM432</t>
+  </si>
+  <si>
+    <t>MODELAGEM DE SOFTWARE COM REDES DE PETRI</t>
+  </si>
+  <si>
+    <t>TM434</t>
+  </si>
+  <si>
+    <t>MINERAÇÃO DE DADOS</t>
+  </si>
+  <si>
+    <t>TM435</t>
+  </si>
+  <si>
+    <t>PROGRAMAÇÃO PARALELA E DISTRIBUÍDA</t>
+  </si>
+  <si>
+    <t>TM436</t>
   </si>
   <si>
     <t>ALGORITMOS PARALELOS E DISTRIBUÍDOS</t>
   </si>
   <si>
+    <t>TM438</t>
+  </si>
+  <si>
+    <t>PROCESSAMENTO DE IMAGENS</t>
+  </si>
+  <si>
+    <t>TM441</t>
+  </si>
+  <si>
+    <t>PROCESSAMENTO DE LINGUAGEM NATURAL</t>
+  </si>
+  <si>
+    <t>TM444</t>
+  </si>
+  <si>
+    <t>BUSCA E RECUPERAÇÃO DE INFORMAÇÃO</t>
+  </si>
+  <si>
+    <t>TN704</t>
+  </si>
+  <si>
+    <t>INTRODUÇÃO À ENGENHARIA DE SOFTWARE EXPERIMENTAL</t>
+  </si>
+  <si>
+    <t>TN708</t>
+  </si>
+  <si>
+    <t>GOVERNANÇA DE TECNOLOGIA DA INFORMAÇÃO</t>
+  </si>
+  <si>
+    <t>TN713</t>
+  </si>
+  <si>
+    <t>INTRODUÇÃO AOS SISTEMAS DE INFORMAÇÃO</t>
+  </si>
+  <si>
+    <t>TN719</t>
+  </si>
+  <si>
+    <t>ENGENHARIA DE SOFTWARE II</t>
+  </si>
+  <si>
+    <t>TN721</t>
+  </si>
+  <si>
+    <t>ARQUITETURA DE SOFTWARE</t>
+  </si>
+  <si>
+    <t>TN722</t>
+  </si>
+  <si>
+    <t>MODELAGEM E ANÁLISE FORMAL DE PROCESSOS DE NEGÓCIO</t>
+  </si>
+  <si>
+    <t>TN732</t>
+  </si>
+  <si>
+    <t>MEDIÇÃO E QUALIDADE DE SOFTWARE</t>
+  </si>
+  <si>
+    <t>TN733</t>
+  </si>
+  <si>
+    <t>INTERAÇÃO HUMANO-COMPUTADOR</t>
+  </si>
+  <si>
+    <t>TN734</t>
+  </si>
+  <si>
+    <t>ENGENHARIA DE REQUISITOS</t>
+  </si>
+  <si>
+    <t>TN735</t>
+  </si>
+  <si>
+    <t>BANCO DE DADOS II</t>
+  </si>
+  <si>
+    <t>TN736</t>
+  </si>
+  <si>
+    <t>INTRODUÇÃO À WEB SEMÂNTICA</t>
+  </si>
+  <si>
+    <t>TN737</t>
+  </si>
+  <si>
+    <t>INTRODUÇÃO À BIOLOGIA COMPUTACIONAL</t>
+  </si>
+  <si>
+    <t>TN739</t>
+  </si>
+  <si>
+    <t>TEORIA DOS JOGOS ALGORÍTMICA</t>
+  </si>
+  <si>
+    <t>TN740</t>
+  </si>
+  <si>
+    <t>TÓPICOS ESPECIAIS EM GRAFOS E ALGORITMOS</t>
+  </si>
+  <si>
+    <t>TN741</t>
+  </si>
+  <si>
+    <t>COMPUTAÇÃO DE ALTO DESEMPENHO</t>
+  </si>
+  <si>
+    <t>TN742</t>
+  </si>
+  <si>
+    <t>PROGRAMAÇÃO EM GPU</t>
+  </si>
+  <si>
+    <t>TN743</t>
+  </si>
+  <si>
+    <t>INTRODUÇÃO À DISPOSITIVOS MÓVEIS</t>
+  </si>
+  <si>
+    <t>TN744</t>
+  </si>
+  <si>
+    <t>ROTEAMENTO EM REDES DE COMPUTADORES</t>
+  </si>
+  <si>
+    <t>TN745</t>
+  </si>
+  <si>
     <t>APRENDIZADO DE MÁQUINA</t>
   </si>
   <si>
+    <t>TN746</t>
+  </si>
+  <si>
+    <t>REDES NEURAIS ARTIFICIAIS</t>
+  </si>
+  <si>
+    <t>TN747</t>
+  </si>
+  <si>
+    <t>INTELIGÊNCIA DE NEGÓCIOS</t>
+  </si>
+  <si>
+    <t>TN748</t>
+  </si>
+  <si>
     <t>ARQUITETURA DE COMPUTADORES II</t>
   </si>
   <si>
-    <t>ARQUITETURA DE SOFTWARE</t>
-  </si>
-  <si>
-    <t>BANCO DE DADOS II</t>
-  </si>
-  <si>
-    <t>BUSCA E RECUPERAÇÃO DE INFORMAÇÃO</t>
-  </si>
-  <si>
-    <t>COMPUTAÇÃO DE ALTO DESEMPENHO</t>
+    <t>TN749</t>
+  </si>
+  <si>
+    <t>TEORIA DOS GRAFOS</t>
+  </si>
+  <si>
+    <t>TN750</t>
+  </si>
+  <si>
+    <t>OTIMIZAÇÃO COMBINATÓRIA</t>
+  </si>
+  <si>
+    <t>TN751</t>
+  </si>
+  <si>
+    <t>TÓPICOS ESPECIAIS EM OTIMIZAÇÃO</t>
+  </si>
+  <si>
+    <t>TN754</t>
   </si>
   <si>
     <t>EMPREENDEDORISMO EM INFORMÁTICA</t>
   </si>
   <si>
-    <t>ENGENHARIA DE REQUISITOS</t>
-  </si>
-  <si>
-    <t>ENGENHARIA DE SOFTWARE II</t>
-  </si>
-  <si>
-    <t>GERÊNCIA DE PROJETOS</t>
+    <t>TN755</t>
   </si>
   <si>
     <t>GESTÃO DE PROCESSOS</t>
-  </si>
-  <si>
-    <t>GOVERNANÇA DE TECNOLOGIA DA INFORMAÇÃO</t>
-  </si>
-  <si>
-    <t>INTELIGÊNCIA DE NEGÓCIOS</t>
-  </si>
-  <si>
-    <t>INTERAÇÃO HUMANO-COMPUTADOR</t>
-  </si>
-  <si>
-    <t>INTRODUÇÃO À BIOLOGIA COMPUTACIONAL</t>
-  </si>
-  <si>
-    <t>INTRODUÇÃO À DISPOSITIVOS MÓVEIS</t>
-  </si>
-  <si>
-    <t>INTRODUÇÃO À ENGENHARIA DE SOFTWARE EXPERIMENTAL</t>
-  </si>
-  <si>
-    <t>INTRODUÇÃO À TEORIA DOS SISTEMAS DE RECOMENDAÇÃO</t>
-  </si>
-  <si>
-    <t>INTRODUÇÃO À TEORIA DAS REDES DE PETRI</t>
-  </si>
-  <si>
-    <t>INTRODUÇÃO À WEB SEMÂNTICA</t>
-  </si>
-  <si>
-    <t>INTRODUÇÃO AOS SISTEMAS DE INFORMAÇÃO</t>
-  </si>
-  <si>
-    <t>MEDIÇÃO E QUALIDADE DE SOFTWARE</t>
-  </si>
-  <si>
-    <t>MINERAÇÃO DE DADOS</t>
-  </si>
-  <si>
-    <t>MODELAGEM DE SOFTWARE COM REDES DE PETRI</t>
-  </si>
-  <si>
-    <t>MODELAGEM E ANÁLISE FORMAL DE PROCESSOS DE NEGÓCIO</t>
-  </si>
-  <si>
-    <t>OTIMIZAÇÃO COMBINATÓRIA</t>
-  </si>
-  <si>
-    <t>PROCESSAMENTO DE IMAGENS</t>
-  </si>
-  <si>
-    <t>PROCESSAMENTO DE LINGUAGEM NATURAL</t>
-  </si>
-  <si>
-    <t>PROGRAMAÇÃO EM GPU</t>
-  </si>
-  <si>
-    <t>PROGRAMAÇÃO PARALELA E DISTRIBUÍDA</t>
-  </si>
-  <si>
-    <t>REDES DE COMPUTADORES SEM FIO</t>
-  </si>
-  <si>
-    <t>REDES NEURAIS ARTIFICIAIS</t>
-  </si>
-  <si>
-    <t>ROTEAMENTO EM REDES DE COMPUTADORES</t>
-  </si>
-  <si>
-    <t>TEORIA DOS GRAFOS</t>
-  </si>
-  <si>
-    <t>TEORIA DOS JOGOS ALGORÍTMICA</t>
-  </si>
-  <si>
-    <t>TÓPICOS ESPECIAIS EM GRAFOS E ALGORITMOS</t>
-  </si>
-  <si>
-    <t>TÓPICOS ESPECIAIS EM OTIMIZAÇÃO</t>
   </si>
 </sst>
 </file>
@@ -277,7 +505,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -286,6 +514,15 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
@@ -506,7 +743,8 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="35.71"/>
+    <col customWidth="1" min="2" max="2" width="44.0"/>
+    <col customWidth="1" min="5" max="5" width="19.29"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -522,894 +760,1080 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1"/>
     </row>
     <row r="2">
-      <c r="A2" s="1">
-        <v>1.0</v>
+      <c r="A2" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1">
         <v>1.0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="4"/>
     </row>
     <row r="3">
-      <c r="A3" s="1">
-        <v>2.0</v>
+      <c r="A3" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1">
         <v>1.0</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="1"/>
     </row>
     <row r="4">
-      <c r="A4" s="1">
-        <v>3.0</v>
+      <c r="A4" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1">
         <v>1.0</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="4"/>
     </row>
     <row r="5">
-      <c r="A5" s="1">
-        <v>4.0</v>
+      <c r="A5" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1">
         <v>1.0</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="4"/>
     </row>
     <row r="6">
-      <c r="A6" s="1">
-        <v>5.0</v>
+      <c r="A6" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1">
         <v>1.0</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="4"/>
     </row>
     <row r="7">
-      <c r="A7" s="1">
-        <v>6.0</v>
+      <c r="A7" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C7" s="1">
         <v>1.0</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="4"/>
     </row>
     <row r="8">
-      <c r="A8" s="1">
-        <v>7.0</v>
+      <c r="A8" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C8" s="1">
         <v>2.0</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="4"/>
     </row>
     <row r="9">
-      <c r="A9" s="1">
-        <v>8.0</v>
+      <c r="A9" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1">
         <v>2.0</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="4"/>
     </row>
     <row r="10">
-      <c r="A10" s="1">
-        <v>9.0</v>
+      <c r="A10" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C10" s="1">
         <v>2.0</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="4"/>
     </row>
     <row r="11">
-      <c r="A11" s="1">
-        <v>10.0</v>
+      <c r="A11" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C11" s="1">
         <v>2.0</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="4"/>
     </row>
     <row r="12">
-      <c r="A12" s="1">
-        <v>11.0</v>
+      <c r="A12" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C12" s="1">
         <v>2.0</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="4"/>
     </row>
     <row r="13">
-      <c r="A13" s="1">
-        <v>12.0</v>
+      <c r="A13" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="C13" s="1">
         <v>2.0</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="F13" s="4"/>
     </row>
     <row r="14">
-      <c r="A14" s="1">
-        <v>13.0</v>
+      <c r="A14" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C14" s="1">
         <v>3.0</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="4"/>
     </row>
     <row r="15">
-      <c r="A15" s="1">
-        <v>14.0</v>
+      <c r="A15" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="C15" s="1">
         <v>3.0</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="4"/>
     </row>
     <row r="16">
-      <c r="A16" s="1">
-        <v>15.0</v>
+      <c r="A16" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="C16" s="1">
         <v>3.0</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16" s="4"/>
     </row>
     <row r="17">
-      <c r="A17" s="1">
-        <v>16.0</v>
+      <c r="A17" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="C17" s="1">
         <v>3.0</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="4"/>
     </row>
     <row r="18">
-      <c r="A18" s="1">
-        <v>17.0</v>
+      <c r="A18" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="C18" s="1">
         <v>3.0</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="4"/>
     </row>
     <row r="19">
-      <c r="A19" s="1">
-        <v>18.0</v>
+      <c r="A19" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="C19" s="1">
         <v>3.0</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E19" s="5"/>
+      <c r="F19" s="4"/>
     </row>
     <row r="20">
-      <c r="A20" s="1">
-        <v>19.0</v>
+      <c r="A20" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="C20" s="1">
         <v>4.0</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" s="4"/>
     </row>
     <row r="21">
-      <c r="A21" s="1">
-        <v>20.0</v>
+      <c r="A21" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="C21" s="1">
         <v>4.0</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E21" s="5"/>
+      <c r="F21" s="4"/>
     </row>
     <row r="22">
-      <c r="A22" s="1">
-        <v>21.0</v>
+      <c r="A22" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="C22" s="1">
         <v>4.0</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F22" s="4"/>
     </row>
     <row r="23">
-      <c r="A23" s="1">
-        <v>22.0</v>
+      <c r="A23" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="C23" s="1">
         <v>4.0</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F23" s="4"/>
     </row>
     <row r="24">
-      <c r="A24" s="1">
-        <v>23.0</v>
+      <c r="A24" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="C24" s="1">
         <v>4.0</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F24" s="4"/>
     </row>
     <row r="25">
-      <c r="A25" s="1">
-        <v>24.0</v>
+      <c r="A25" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="C25" s="1">
         <v>4.0</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F25" s="4"/>
     </row>
     <row r="26">
-      <c r="A26" s="1">
-        <v>25.0</v>
+      <c r="A26" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="C26" s="1">
         <v>5.0</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F26" s="4"/>
     </row>
     <row r="27">
-      <c r="A27" s="1">
-        <v>26.0</v>
+      <c r="A27" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="C27" s="1">
         <v>5.0</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F27" s="4"/>
     </row>
     <row r="28">
-      <c r="A28" s="1">
-        <v>27.0</v>
+      <c r="A28" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="C28" s="1">
         <v>5.0</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F28" s="4"/>
     </row>
     <row r="29">
-      <c r="A29" s="1">
-        <v>28.0</v>
+      <c r="A29" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="C29" s="1">
         <v>5.0</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F29" s="4"/>
     </row>
     <row r="30">
-      <c r="A30" s="1">
-        <v>29.0</v>
+      <c r="A30" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="C30" s="1">
         <v>5.0</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E30" s="5"/>
+      <c r="F30" s="4"/>
     </row>
     <row r="31">
-      <c r="A31" s="1">
-        <v>30.0</v>
+      <c r="A31" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="C31" s="1">
         <v>5.0</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F31" s="4"/>
     </row>
     <row r="32">
-      <c r="A32" s="1">
-        <v>31.0</v>
+      <c r="A32" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="C32" s="1">
         <v>6.0</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F32" s="4"/>
     </row>
     <row r="33">
-      <c r="A33" s="1">
-        <v>32.0</v>
+      <c r="A33" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="C33" s="1">
         <v>6.0</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F33" s="4"/>
     </row>
     <row r="34">
-      <c r="A34" s="1">
-        <v>33.0</v>
+      <c r="A34" s="6" t="s">
+        <v>73</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>38</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
     </row>
     <row r="35">
-      <c r="A35" s="1">
-        <v>34.0</v>
+      <c r="A35" s="6" t="s">
+        <v>76</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>39</v>
+        <v>77</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
     </row>
     <row r="36">
-      <c r="A36" s="1">
-        <v>35.0</v>
+      <c r="A36" s="6" t="s">
+        <v>78</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>40</v>
+        <v>79</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
     </row>
     <row r="37">
-      <c r="A37" s="1">
-        <v>36.0</v>
+      <c r="A37" s="6" t="s">
+        <v>80</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>41</v>
+        <v>81</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
     </row>
     <row r="38">
-      <c r="A38" s="1">
-        <v>37.0</v>
+      <c r="A38" s="6" t="s">
+        <v>82</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>42</v>
+        <v>83</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
     </row>
     <row r="39">
-      <c r="A39" s="1">
-        <v>38.0</v>
+      <c r="A39" s="6" t="s">
+        <v>84</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>43</v>
+        <v>85</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
     </row>
     <row r="40">
-      <c r="A40" s="1">
-        <v>39.0</v>
+      <c r="A40" s="6" t="s">
+        <v>86</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>44</v>
+        <v>87</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
     </row>
     <row r="41">
-      <c r="A41" s="1">
-        <v>40.0</v>
+      <c r="A41" s="6" t="s">
+        <v>88</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>45</v>
+        <v>89</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
     </row>
     <row r="42">
-      <c r="A42" s="1">
-        <v>41.0</v>
+      <c r="A42" s="6" t="s">
+        <v>90</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>46</v>
+        <v>91</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
     </row>
     <row r="43">
-      <c r="A43" s="1">
-        <v>42.0</v>
+      <c r="A43" s="6" t="s">
+        <v>92</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>47</v>
+        <v>93</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
     </row>
     <row r="44">
-      <c r="A44" s="1">
-        <v>43.0</v>
+      <c r="A44" s="6" t="s">
+        <v>94</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>48</v>
+        <v>95</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
     </row>
     <row r="45">
-      <c r="A45" s="1">
-        <v>44.0</v>
+      <c r="A45" s="6" t="s">
+        <v>96</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>49</v>
+        <v>97</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
     </row>
     <row r="46">
-      <c r="A46" s="1">
-        <v>45.0</v>
+      <c r="A46" s="6" t="s">
+        <v>98</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
     </row>
     <row r="47">
-      <c r="A47" s="1">
-        <v>46.0</v>
+      <c r="A47" s="6" t="s">
+        <v>100</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
     </row>
     <row r="48">
-      <c r="A48" s="1">
-        <v>47.0</v>
+      <c r="A48" s="6" t="s">
+        <v>102</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>52</v>
+        <v>103</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
     </row>
     <row r="49">
-      <c r="A49" s="1">
-        <v>48.0</v>
+      <c r="A49" s="6" t="s">
+        <v>104</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>53</v>
+        <v>105</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
     </row>
     <row r="50">
-      <c r="A50" s="1">
-        <v>49.0</v>
+      <c r="A50" s="6" t="s">
+        <v>106</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>54</v>
+        <v>107</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
     </row>
     <row r="51">
-      <c r="A51" s="1">
-        <v>50.0</v>
+      <c r="A51" s="6" t="s">
+        <v>108</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>55</v>
+        <v>109</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
     </row>
     <row r="52">
-      <c r="A52" s="1">
-        <v>51.0</v>
+      <c r="A52" s="6" t="s">
+        <v>110</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>56</v>
+        <v>111</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
     </row>
     <row r="53">
-      <c r="A53" s="1">
-        <v>52.0</v>
+      <c r="A53" s="6" t="s">
+        <v>112</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>57</v>
+        <v>113</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
     </row>
     <row r="54">
-      <c r="A54" s="1">
-        <v>53.0</v>
+      <c r="A54" s="6" t="s">
+        <v>114</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>58</v>
+        <v>115</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
     </row>
     <row r="55">
-      <c r="A55" s="1">
-        <v>54.0</v>
+      <c r="A55" s="6" t="s">
+        <v>116</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>59</v>
+        <v>117</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
     </row>
     <row r="56">
-      <c r="A56" s="1">
-        <v>55.0</v>
+      <c r="A56" s="6" t="s">
+        <v>118</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>60</v>
+        <v>119</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E56" s="4"/>
+      <c r="F56" s="4"/>
     </row>
     <row r="57">
-      <c r="A57" s="1">
-        <v>56.0</v>
+      <c r="A57" s="6" t="s">
+        <v>120</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>61</v>
+        <v>121</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
     </row>
     <row r="58">
-      <c r="A58" s="1">
-        <v>57.0</v>
+      <c r="A58" s="6" t="s">
+        <v>122</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>62</v>
+        <v>123</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E58" s="4"/>
+      <c r="F58" s="4"/>
     </row>
     <row r="59">
-      <c r="A59" s="1">
-        <v>58.0</v>
+      <c r="A59" s="6" t="s">
+        <v>124</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>63</v>
+        <v>125</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E59" s="4"/>
+      <c r="F59" s="4"/>
     </row>
     <row r="60">
-      <c r="A60" s="1">
-        <v>59.0</v>
+      <c r="A60" s="6" t="s">
+        <v>126</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>64</v>
+        <v>127</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
     </row>
     <row r="61">
-      <c r="A61" s="1">
-        <v>60.0</v>
+      <c r="A61" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>65</v>
+        <v>129</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E61" s="4"/>
+      <c r="F61" s="4"/>
     </row>
     <row r="62">
-      <c r="A62" s="1">
-        <v>61.0</v>
+      <c r="A62" s="6" t="s">
+        <v>130</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>66</v>
+        <v>131</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4"/>
     </row>
     <row r="63">
-      <c r="A63" s="1">
-        <v>62.0</v>
+      <c r="A63" s="6" t="s">
+        <v>132</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>67</v>
+        <v>133</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E63" s="4"/>
+      <c r="F63" s="4"/>
     </row>
     <row r="64">
-      <c r="A64" s="1">
-        <v>63.0</v>
+      <c r="A64" s="6" t="s">
+        <v>134</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>68</v>
+        <v>135</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E64" s="4"/>
+      <c r="F64" s="4"/>
     </row>
     <row r="65">
-      <c r="A65" s="1">
-        <v>64.0</v>
+      <c r="A65" s="6" t="s">
+        <v>136</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>69</v>
+        <v>137</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E65" s="4"/>
+      <c r="F65" s="4"/>
     </row>
     <row r="66">
-      <c r="A66" s="1">
-        <v>65.0</v>
+      <c r="A66" s="6" t="s">
+        <v>138</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>70</v>
+        <v>139</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E66" s="4"/>
+      <c r="F66" s="4"/>
     </row>
     <row r="67">
-      <c r="A67" s="1">
-        <v>66.0</v>
+      <c r="A67" s="6" t="s">
+        <v>140</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>71</v>
+        <v>141</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E67" s="4"/>
+      <c r="F67" s="4"/>
     </row>
     <row r="68">
-      <c r="A68" s="1">
-        <v>67.0</v>
+      <c r="A68" s="6" t="s">
+        <v>142</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>72</v>
+        <v>143</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E68" s="4"/>
+      <c r="F68" s="4"/>
     </row>
     <row r="69">
-      <c r="A69" s="1">
-        <v>68.0</v>
+      <c r="A69" s="6" t="s">
+        <v>144</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>73</v>
+        <v>145</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E69" s="4"/>
+      <c r="F69" s="4"/>
     </row>
     <row r="70">
-      <c r="A70" s="1">
-        <v>69.0</v>
+      <c r="A70" s="6" t="s">
+        <v>146</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>74</v>
+        <v>147</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E70" s="4"/>
+      <c r="F70" s="4"/>
     </row>
     <row r="71">
-      <c r="A71" s="1">
-        <v>70.0</v>
+      <c r="A71" s="6" t="s">
+        <v>148</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>75</v>
+        <v>149</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E71" s="4"/>
+      <c r="F71" s="4"/>
     </row>
     <row r="72">
-      <c r="A72" s="1">
-        <v>71.0</v>
+      <c r="A72" s="6" t="s">
+        <v>150</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>76</v>
+        <v>151</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E72" s="4"/>
+      <c r="F72" s="4"/>
     </row>
     <row r="73">
-      <c r="A73" s="1">
-        <v>72.0</v>
+      <c r="A73" s="6" t="s">
+        <v>152</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>77</v>
+        <v>153</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E73" s="4"/>
+      <c r="F73" s="4"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>